<commit_message>
Update tests for manegeplan change
</commit_message>
<xml_diff>
--- a/tests/manegeplan-export.xlsx
+++ b/tests/manegeplan-export.xlsx
@@ -13,19 +13,19 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="13">
   <si>
-    <t>Voornaam</t>
+    <t>Roepnaam</t>
   </si>
   <si>
-    <t>Tussen</t>
+    <t>Tussenvoegsels</t>
   </si>
   <si>
     <t>Achternaam</t>
   </si>
   <si>
-    <t>Email</t>
+    <t>E_Mail</t>
   </si>
   <si>
-    <t>Gebruiker_id</t>
+    <t>Persoon_ID</t>
   </si>
   <si>
     <t>Alice</t>
@@ -96,7 +96,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -111,12 +111,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor indexed="13"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -251,13 +257,100 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="12"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="12"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="12"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="12"/>
+      </right>
+      <top style="thin">
+        <color indexed="12"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="12"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="12"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="12"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="12"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="12"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="12"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="12"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -265,42 +358,72 @@
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+      <alignment vertical="bottom" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -524,17 +647,17 @@
         <a:solidFill>
           <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -561,10 +684,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -803,12 +926,12 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -1085,7 +1208,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1112,10 +1235,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1357,7 +1480,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1379,56 +1502,104 @@
       <c r="B1" t="s" s="3">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="3">
+      <c r="C1" t="s" s="4">
         <v>2</v>
       </c>
       <c r="D1" t="s" s="3">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="4">
+      <c r="E1" t="s" s="5">
         <v>4</v>
       </c>
-      <c r="F1" s="5"/>
+      <c r="F1" s="6"/>
     </row>
     <row r="2" ht="13.55" customHeight="1">
-      <c r="A2" t="s" s="6">
+      <c r="A2" t="s" s="7">
         <v>5</v>
       </c>
-      <c r="B2" t="s" s="7">
+      <c r="B2" t="s" s="8">
         <v>6</v>
       </c>
-      <c r="C2" t="s" s="7">
+      <c r="C2" t="s" s="8">
         <v>7</v>
       </c>
-      <c r="D2" t="s" s="7">
+      <c r="D2" t="s" s="8">
         <v>8</v>
       </c>
-      <c r="E2" t="s" s="8">
+      <c r="E2" t="s" s="9">
         <v>9</v>
       </c>
-      <c r="F2" s="5"/>
+      <c r="F2" s="6"/>
     </row>
     <row r="3" ht="13.55" customHeight="1">
-      <c r="A3" t="s" s="9">
+      <c r="A3" t="s" s="10">
         <v>10</v>
       </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" t="s" s="11">
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" t="s" s="12">
         <v>11</v>
       </c>
-      <c r="E3" t="s" s="12">
+      <c r="E3" t="s" s="13">
         <v>12</v>
       </c>
-      <c r="F3" s="5"/>
+      <c r="F3" s="6"/>
     </row>
     <row r="4" ht="13.55" customHeight="1">
-      <c r="A4" s="13"/>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="14"/>
+      <c r="A4" s="14"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="15"/>
+    </row>
+    <row r="5" ht="13.55" customHeight="1">
+      <c r="A5" s="16"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="18"/>
+    </row>
+    <row r="6" ht="13.55" customHeight="1">
+      <c r="A6" s="19"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="21"/>
+    </row>
+    <row r="7" ht="13.55" customHeight="1">
+      <c r="A7" s="19"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="21"/>
+    </row>
+    <row r="8" ht="13.55" customHeight="1">
+      <c r="A8" s="19"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="21"/>
+    </row>
+    <row r="9" ht="13.55" customHeight="1">
+      <c r="A9" s="19"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="21"/>
+    </row>
+    <row r="10" ht="13.55" customHeight="1">
+      <c r="A10" s="22"/>
+      <c r="B10" s="23"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="24"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Update for changed manegeplan export (#8)
</commit_message>
<xml_diff>
--- a/tests/manegeplan-export.xlsx
+++ b/tests/manegeplan-export.xlsx
@@ -13,19 +13,19 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="13">
   <si>
-    <t>Voornaam</t>
+    <t>Roepnaam</t>
   </si>
   <si>
-    <t>Tussen</t>
+    <t>Tussenvoegsels</t>
   </si>
   <si>
     <t>Achternaam</t>
   </si>
   <si>
-    <t>Email</t>
+    <t>E_Mail</t>
   </si>
   <si>
-    <t>Gebruiker_id</t>
+    <t>Persoon_ID</t>
   </si>
   <si>
     <t>Alice</t>
@@ -96,7 +96,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -111,12 +111,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor indexed="13"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -251,13 +257,100 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="12"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="12"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="12"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="12"/>
+      </right>
+      <top style="thin">
+        <color indexed="12"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="12"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="12"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="12"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="12"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="12"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="12"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="12"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -265,42 +358,72 @@
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+      <alignment vertical="bottom" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -524,17 +647,17 @@
         <a:solidFill>
           <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -561,10 +684,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -803,12 +926,12 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -1085,7 +1208,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1112,10 +1235,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1357,7 +1480,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1379,56 +1502,104 @@
       <c r="B1" t="s" s="3">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="3">
+      <c r="C1" t="s" s="4">
         <v>2</v>
       </c>
       <c r="D1" t="s" s="3">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="4">
+      <c r="E1" t="s" s="5">
         <v>4</v>
       </c>
-      <c r="F1" s="5"/>
+      <c r="F1" s="6"/>
     </row>
     <row r="2" ht="13.55" customHeight="1">
-      <c r="A2" t="s" s="6">
+      <c r="A2" t="s" s="7">
         <v>5</v>
       </c>
-      <c r="B2" t="s" s="7">
+      <c r="B2" t="s" s="8">
         <v>6</v>
       </c>
-      <c r="C2" t="s" s="7">
+      <c r="C2" t="s" s="8">
         <v>7</v>
       </c>
-      <c r="D2" t="s" s="7">
+      <c r="D2" t="s" s="8">
         <v>8</v>
       </c>
-      <c r="E2" t="s" s="8">
+      <c r="E2" t="s" s="9">
         <v>9</v>
       </c>
-      <c r="F2" s="5"/>
+      <c r="F2" s="6"/>
     </row>
     <row r="3" ht="13.55" customHeight="1">
-      <c r="A3" t="s" s="9">
+      <c r="A3" t="s" s="10">
         <v>10</v>
       </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" t="s" s="11">
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" t="s" s="12">
         <v>11</v>
       </c>
-      <c r="E3" t="s" s="12">
+      <c r="E3" t="s" s="13">
         <v>12</v>
       </c>
-      <c r="F3" s="5"/>
+      <c r="F3" s="6"/>
     </row>
     <row r="4" ht="13.55" customHeight="1">
-      <c r="A4" s="13"/>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="14"/>
+      <c r="A4" s="14"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="15"/>
+    </row>
+    <row r="5" ht="13.55" customHeight="1">
+      <c r="A5" s="16"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="18"/>
+    </row>
+    <row r="6" ht="13.55" customHeight="1">
+      <c r="A6" s="19"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="21"/>
+    </row>
+    <row r="7" ht="13.55" customHeight="1">
+      <c r="A7" s="19"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="21"/>
+    </row>
+    <row r="8" ht="13.55" customHeight="1">
+      <c r="A8" s="19"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="21"/>
+    </row>
+    <row r="9" ht="13.55" customHeight="1">
+      <c r="A9" s="19"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="21"/>
+    </row>
+    <row r="10" ht="13.55" customHeight="1">
+      <c r="A10" s="22"/>
+      <c r="B10" s="23"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="24"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>